<commit_message>
add method to convert letter column into openpyxl understandable column
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Python\excelToDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5273210-D325-441E-BAB3-B371DA7334B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F0D625-BC80-4DC2-8755-838CA22F2C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="1995" windowWidth="20910" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>B2</t>
   </si>
@@ -98,6 +98,24 @@
   </si>
   <si>
     <t>c4</t>
+  </si>
+  <si>
+    <t>c5</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
   </si>
 </sst>
 </file>
@@ -422,15 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -446,8 +464,11 @@
       <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -463,8 +484,11 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -480,8 +504,11 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -497,8 +524,11 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -514,8 +544,11 @@
       <c r="E5" t="s">
         <v>17</v>
       </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -530,6 +563,9 @@
       </c>
       <c r="E6" t="s">
         <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ead the dictionary inputed by user, assemble sql query and insert to the database line by line according to the user inputed dictionary
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Python\excelToDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F0D625-BC80-4DC2-8755-838CA22F2C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2017AEA7-4184-4BE8-A7BE-E034C76E6298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,14 +443,14 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -489,8 +489,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" s="1">
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -529,8 +529,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" s="1">
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Compile python model to dll let C++/C# program load it
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Python\excelToDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2017AEA7-4184-4BE8-A7BE-E034C76E6298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD24BF6B-D10A-45F6-8A71-CBF529E975EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>c4</t>
   </si>
   <si>
-    <t>c5</t>
-  </si>
-  <si>
     <t>F2</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>F6</t>
+  </si>
+  <si>
+    <t>F1</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +465,7 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -485,7 +485,7 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -505,7 +505,7 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -525,7 +525,7 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -545,7 +545,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>